<commit_message>
Add contacted on dates
</commit_message>
<xml_diff>
--- a/MediaOutlist.xlsx
+++ b/MediaOutlist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -68,9 +68,6 @@
     <t>http://forums.hackaday.com/</t>
   </si>
   <si>
-    <t>editor@makezine.com</t>
-  </si>
-  <si>
     <t>info@oshwa.org</t>
   </si>
   <si>
@@ -158,30 +155,6 @@
     <t>alex.hern@theguardian.com</t>
   </si>
   <si>
-    <t>Stuart Dredge</t>
-  </si>
-  <si>
-    <t>stuart.dredge@theguardian.com</t>
-  </si>
-  <si>
-    <t>Paul Boyd, Multimedia editor</t>
-  </si>
-  <si>
-    <t>paul.boyd@theguardian.com</t>
-  </si>
-  <si>
-    <t>Jason Phipps, Audio producer</t>
-  </si>
-  <si>
-    <t>jason.phipps@theguardian.com</t>
-  </si>
-  <si>
-    <t>Martyn Dore, Administrator</t>
-  </si>
-  <si>
-    <t>martyn.dore@theguardian.com</t>
-  </si>
-  <si>
     <t>Bianca@huffingtonpost.com</t>
   </si>
   <si>
@@ -191,9 +164,6 @@
     <t>tips@tested.com</t>
   </si>
   <si>
-    <t>Emailed On</t>
-  </si>
-  <si>
     <t>See Sheet 2</t>
   </si>
   <si>
@@ -345,6 +315,18 @@
   </si>
   <si>
     <t>Luke Nozicka, Campus Editor</t>
+  </si>
+  <si>
+    <t>Contacted On</t>
+  </si>
+  <si>
+    <t>New Blankets</t>
+  </si>
+  <si>
+    <t>Arch Reactor</t>
+  </si>
+  <si>
+    <t>Open Space SI</t>
   </si>
 </sst>
 </file>
@@ -744,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +738,7 @@
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -770,10 +752,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,13 +765,16 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E2" s="3">
+        <v>41913</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -802,16 +787,20 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E4" s="3">
+        <v>41913</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
+      </c>
+      <c r="E5" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -819,7 +808,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -827,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -835,7 +827,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>93</v>
+      </c>
+      <c r="E8" s="3">
+        <v>41912</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,7 +838,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,7 +846,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E10" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -859,10 +857,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -870,71 +868,95 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="E12" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E13" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+      <c r="E14" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E15" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E16" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>86</v>
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="E18" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="E19" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E20" s="3">
         <v>41912</v>
@@ -942,66 +964,111 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="E21" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="E22" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>70</v>
+      </c>
+      <c r="E23" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>75</v>
+      </c>
+      <c r="E24" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="E25" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>87</v>
+      </c>
+      <c r="E26" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>89</v>
+      </c>
+      <c r="E27" s="3">
+        <v>41913</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="3">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>101</v>
+      </c>
+      <c r="E29" s="3">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="3">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1010,15 +1077,14 @@
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4" display="http://makezine.com/forums/"/>
-    <hyperlink ref="B5" r:id="rId5" display="mailto:editor@makezine.com"/>
-    <hyperlink ref="B6" r:id="rId6" display="mailto:info@oshwa.org"/>
-    <hyperlink ref="C7" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B20" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId5" display="mailto:info@oshwa.org"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B20" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1026,227 +1092,195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>